<commit_message>
Author:Author    : Pooja Sharma Files Added      : PoojaSharma.xlsx Description      : Replaced the previous existing PoojaSharma.xlsx
</commit_message>
<xml_diff>
--- a/TeamDetails/TasksBreakDown/PoojaSharma.xlsx
+++ b/TeamDetails/TasksBreakDown/PoojaSharma.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="43">
   <si>
     <t>Story ID</t>
   </si>
@@ -59,18 +59,6 @@
     <t>Add clickable image in Last Column(view File) of  Ui-grid table</t>
   </si>
   <si>
-    <t>Creating Yml and Configsql file</t>
-  </si>
-  <si>
-    <t>Creating Dto and Dao</t>
-  </si>
-  <si>
-    <t>Creating Controllers and Services</t>
-  </si>
-  <si>
-    <t>Creating a dummy databse and Create JDBC connection</t>
-  </si>
-  <si>
     <t>Write logic of on-click image functionality i.e, view uploaded excel file,  in services</t>
   </si>
   <si>
@@ -81,9 +69,6 @@
   </si>
   <si>
     <t>SSDMS-47&amp;48</t>
-  </si>
-  <si>
-    <t>Integrate the front end code with backend.</t>
   </si>
   <si>
     <t>T-1</t>
@@ -203,9 +188,6 @@
     <t>Unit Testing</t>
   </si>
   <si>
-    <t>T-13</t>
-  </si>
-  <si>
     <t>Rework</t>
   </si>
   <si>
@@ -216,13 +198,28 @@
   </si>
   <si>
     <t>Block Diagrams of the whole journey</t>
+  </si>
+  <si>
+    <t>Establish Database connection</t>
+  </si>
+  <si>
+    <t>Populate values on the frontend</t>
+  </si>
+  <si>
+    <t>Create a dummy table in the Database</t>
+  </si>
+  <si>
+    <t>Receive Values from the Database</t>
+  </si>
+  <si>
+    <t>Integrate the Code</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -239,6 +236,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
@@ -246,8 +250,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="9" tint="0.79998168889431442"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="9" tint="0.59999389629810485"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -262,19 +280,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.79998168889431442"/>
+        <fgColor theme="8" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -284,20 +302,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="5">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -320,48 +326,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -376,56 +345,49 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -434,6 +396,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFFCCFF"/>
+      <color rgb="FFFF9966"/>
+      <color rgb="FFFF99FF"/>
+      <color rgb="FFCC66FF"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -708,10 +678,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G63"/>
+  <dimension ref="A1:I63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -748,408 +718,409 @@
       </c>
     </row>
     <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="21"/>
-      <c r="B2" s="21"/>
-      <c r="C2" s="21"/>
-      <c r="D2" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="E2" s="21"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2">
+      <c r="A2" s="18"/>
+      <c r="B2" s="18"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2" s="18"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22">
         <f>E2-F2</f>
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="21"/>
-      <c r="B3" s="21"/>
-      <c r="C3" s="21"/>
-      <c r="D3" s="12"/>
+      <c r="A3" s="18"/>
+      <c r="B3" s="18"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="10"/>
       <c r="E3" s="21"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
+      <c r="F3" s="22"/>
+      <c r="G3" s="22"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="21"/>
-      <c r="B4" s="21"/>
-      <c r="C4" s="21"/>
-      <c r="D4" s="12" t="s">
+      <c r="A4" s="18"/>
+      <c r="B4" s="18"/>
+      <c r="C4" s="18"/>
+      <c r="D4" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4" s="21"/>
+      <c r="F4" s="22"/>
+      <c r="G4" s="22"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="18"/>
+      <c r="B5" s="18"/>
+      <c r="C5" s="18"/>
+      <c r="D5" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5" s="21"/>
+      <c r="F5" s="22"/>
+      <c r="G5" s="22"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="18"/>
+      <c r="B6" s="18"/>
+      <c r="C6" s="18"/>
+      <c r="D6" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" s="21"/>
+      <c r="F6" s="22"/>
+      <c r="G6" s="22"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="18"/>
+      <c r="B7" s="18"/>
+      <c r="C7" s="18"/>
+      <c r="D7" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" s="21"/>
+      <c r="F7" s="22"/>
+      <c r="G7" s="22"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="18"/>
+      <c r="B8" s="18"/>
+      <c r="C8" s="18"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="21"/>
+      <c r="F8" s="22"/>
+      <c r="G8" s="22"/>
+    </row>
+    <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="18"/>
+      <c r="B9" s="18"/>
+      <c r="C9" s="18"/>
+      <c r="D9" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="E4" s="21"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="21"/>
-      <c r="B5" s="21"/>
-      <c r="C5" s="21"/>
-      <c r="D5" s="19" t="s">
-        <v>31</v>
-      </c>
-      <c r="E5" s="21"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="21"/>
-      <c r="B6" s="21"/>
-      <c r="C6" s="21"/>
-      <c r="D6" s="19" t="s">
-        <v>34</v>
-      </c>
-      <c r="E6" s="21"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="21"/>
-      <c r="B7" s="21"/>
-      <c r="C7" s="21"/>
-      <c r="D7" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="E7" s="21"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="21"/>
-      <c r="B8" s="21"/>
-      <c r="C8" s="21"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="21"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-    </row>
-    <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="21"/>
-      <c r="B9" s="21"/>
-      <c r="C9" s="21"/>
-      <c r="D9" s="12" t="s">
-        <v>35</v>
-      </c>
       <c r="E9" s="21"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
+      <c r="F9" s="22"/>
+      <c r="G9" s="22"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="21"/>
-      <c r="B10" s="21"/>
-      <c r="C10" s="21"/>
-      <c r="D10" s="12"/>
+      <c r="A10" s="18"/>
+      <c r="B10" s="18"/>
+      <c r="C10" s="18"/>
+      <c r="D10" s="10"/>
       <c r="E10" s="21"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
+      <c r="F10" s="22"/>
+      <c r="G10" s="22"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="21"/>
-      <c r="B11" s="21"/>
-      <c r="C11" s="21"/>
-      <c r="D11" s="20" t="s">
-        <v>43</v>
+      <c r="A11" s="18"/>
+      <c r="B11" s="18"/>
+      <c r="C11" s="18"/>
+      <c r="D11" s="19" t="s">
+        <v>37</v>
       </c>
       <c r="E11" s="21"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
+      <c r="F11" s="22"/>
+      <c r="G11" s="22"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="21"/>
-      <c r="B12" s="21"/>
-      <c r="C12" s="21"/>
+      <c r="A12" s="18"/>
+      <c r="B12" s="18"/>
+      <c r="C12" s="18"/>
       <c r="D12" s="14"/>
       <c r="E12" s="21"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
+      <c r="F12" s="22"/>
+      <c r="G12" s="22"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="B13" s="16">
+      <c r="A13" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="23">
         <v>22</v>
       </c>
-      <c r="C13" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D13" s="7" t="s">
+      <c r="C13" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="E13" s="6">
+      <c r="E13" s="7">
         <v>2</v>
       </c>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2">
+      <c r="F13" s="17"/>
+      <c r="G13" s="17">
         <f>E13-F13</f>
         <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="17"/>
-      <c r="B14" s="17"/>
-      <c r="C14" s="6" t="s">
-        <v>21</v>
+      <c r="A14" s="23"/>
+      <c r="B14" s="23"/>
+      <c r="C14" s="7" t="s">
+        <v>16</v>
       </c>
       <c r="D14" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="E14" s="6">
-        <v>1</v>
-      </c>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2">
+      <c r="E14" s="7">
+        <v>1</v>
+      </c>
+      <c r="F14" s="17"/>
+      <c r="G14" s="17">
         <f t="shared" ref="G14:G63" si="0">E14-F14</f>
         <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="17"/>
-      <c r="B15" s="17"/>
-      <c r="C15" s="6" t="s">
-        <v>22</v>
+      <c r="A15" s="23"/>
+      <c r="B15" s="23"/>
+      <c r="C15" s="7" t="s">
+        <v>17</v>
       </c>
       <c r="D15" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="E15" s="6">
-        <v>1</v>
-      </c>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2">
+      <c r="E15" s="7">
+        <v>1</v>
+      </c>
+      <c r="F15" s="17"/>
+      <c r="G15" s="17">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="17"/>
-      <c r="B16" s="17"/>
-      <c r="C16" s="6" t="s">
-        <v>23</v>
+      <c r="A16" s="23"/>
+      <c r="B16" s="23"/>
+      <c r="C16" s="7" t="s">
+        <v>18</v>
       </c>
       <c r="D16" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="E16" s="6">
-        <v>1</v>
-      </c>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="17"/>
-      <c r="B17" s="17"/>
-      <c r="C17" s="6" t="s">
+      <c r="E16" s="7">
+        <v>1</v>
+      </c>
+      <c r="F16" s="17"/>
+      <c r="G16" s="17">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="23"/>
+      <c r="B17" s="23"/>
+      <c r="C17" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="E17" s="7">
+        <v>2</v>
+      </c>
+      <c r="F17" s="17"/>
+      <c r="G17" s="17">
+        <f t="shared" ref="G17:G18" si="1">E17-F17</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="23"/>
+      <c r="B18" s="23"/>
+      <c r="C18" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="E18" s="7">
+        <v>1</v>
+      </c>
+      <c r="F18" s="17"/>
+      <c r="G18" s="17">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="23"/>
+      <c r="B19" s="23"/>
+      <c r="C19" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="E19" s="7">
+        <v>1</v>
+      </c>
+      <c r="F19" s="17"/>
+      <c r="G19" s="17">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="23"/>
+      <c r="B20" s="23"/>
+      <c r="C20" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D20" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="E20" s="7">
+        <v>1</v>
+      </c>
+      <c r="F20" s="17"/>
+      <c r="G20" s="17">
+        <v>1</v>
+      </c>
+      <c r="I20" s="6"/>
+    </row>
+    <row r="21" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="23"/>
+      <c r="B21" s="23"/>
+      <c r="C21" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D21" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E21" s="7">
+        <v>6</v>
+      </c>
+      <c r="F21" s="17"/>
+      <c r="G21" s="17">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="23"/>
+      <c r="B22" s="23"/>
+      <c r="C22" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D22" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="E22" s="7">
+        <v>2</v>
+      </c>
+      <c r="F22" s="17"/>
+      <c r="G22" s="17">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="23"/>
+      <c r="B23" s="23"/>
+      <c r="C23" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="D17" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="E17" s="6">
+      <c r="D23" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="E23" s="7">
+        <v>1</v>
+      </c>
+      <c r="F23" s="17"/>
+      <c r="G23" s="17">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="23"/>
+      <c r="B24" s="23"/>
+      <c r="C24" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="D24" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="E24" s="7">
+        <v>1</v>
+      </c>
+      <c r="F24" s="17"/>
+      <c r="G24" s="17">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" s="23"/>
+      <c r="B25" s="23"/>
+      <c r="C25" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="D25" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="E25" s="7">
         <v>2</v>
       </c>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2">
-        <f t="shared" ref="G17" si="1">E17-F17</f>
+      <c r="F25" s="17"/>
+      <c r="G25" s="17">
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="17"/>
-      <c r="B18" s="17"/>
-      <c r="C18" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="D18" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="E18" s="6">
-        <v>1</v>
-      </c>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="17"/>
-      <c r="B19" s="17"/>
-      <c r="C19" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="D19" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="E19" s="6">
-        <v>1</v>
-      </c>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="17"/>
-      <c r="B20" s="17"/>
-      <c r="C20" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="D20" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="E20" s="6">
-        <v>1</v>
-      </c>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="17"/>
-      <c r="B21" s="17"/>
-      <c r="C21" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="D21" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="E21" s="6">
-        <v>6</v>
-      </c>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="17"/>
-      <c r="B22" s="17"/>
-      <c r="C22" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="D22" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="E22" s="6">
-        <v>2</v>
-      </c>
-      <c r="F22" s="2"/>
-      <c r="G22" s="2">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="17"/>
-      <c r="B23" s="17"/>
-      <c r="C23" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="D23" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="E23" s="6">
-        <v>1</v>
-      </c>
-      <c r="F23" s="2"/>
-      <c r="G23" s="2">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="17"/>
-      <c r="B24" s="17"/>
-      <c r="C24" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="D24" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="E24" s="6">
-        <v>1</v>
-      </c>
-      <c r="F24" s="2"/>
-      <c r="G24" s="2">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="18"/>
-      <c r="B25" s="18"/>
-      <c r="C25" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="D25" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="E25" s="6">
-        <v>2</v>
-      </c>
-      <c r="F25" s="2"/>
-      <c r="G25" s="2">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="21"/>
-      <c r="B26" s="21"/>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" s="18"/>
+      <c r="B26" s="18"/>
       <c r="C26" s="15"/>
       <c r="D26" s="14"/>
       <c r="E26" s="13"/>
-      <c r="F26" s="2"/>
-      <c r="G26" s="2"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="22" t="s">
+      <c r="F26" s="21"/>
+      <c r="G26" s="21"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="B27" s="24">
+        <v>8</v>
+      </c>
+      <c r="C27" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="D27" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="E27" s="11">
+        <v>4</v>
+      </c>
+      <c r="F27" s="16"/>
+      <c r="G27" s="16">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" s="24"/>
+      <c r="B28" s="24"/>
+      <c r="C28" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="B27" s="22">
-        <v>8</v>
-      </c>
-      <c r="C27" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="D27" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="E27" s="10">
+      <c r="D28" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="E28" s="11">
         <v>4</v>
       </c>
-      <c r="F27" s="2"/>
-      <c r="G27" s="2">
+      <c r="F28" s="16"/>
+      <c r="G28" s="16">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="23"/>
-      <c r="B28" s="23"/>
-      <c r="C28" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="D28" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="E28" s="10">
-        <v>4</v>
-      </c>
-      <c r="F28" s="2"/>
-      <c r="G28" s="2">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="2"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
@@ -1161,7 +1132,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="2"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
@@ -1173,7 +1144,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="2"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
@@ -1185,7 +1156,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="2"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>

</xml_diff>

<commit_message>
Author           : Pooja Sharma Files Added      : PoojaSharma.xlsx Description      : Replaced the previous existing PoojaSharma.xlsx
</commit_message>
<xml_diff>
--- a/TeamDetails/TasksBreakDown/PoojaSharma.xlsx
+++ b/TeamDetails/TasksBreakDown/PoojaSharma.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pooja sharma\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\New folder\trunk\TeamDetails\TasksBreakDown\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="44">
   <si>
     <t>Story ID</t>
   </si>
@@ -213,6 +213,9 @@
   </si>
   <si>
     <t>Integrate the Code</t>
+  </si>
+  <si>
+    <t>T-13</t>
   </si>
 </sst>
 </file>
@@ -680,8 +683,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -949,7 +952,7 @@
       <c r="A19" s="23"/>
       <c r="B19" s="23"/>
       <c r="C19" s="7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D19" s="8" t="s">
         <v>41</v>
@@ -967,7 +970,7 @@
       <c r="A20" s="23"/>
       <c r="B20" s="23"/>
       <c r="C20" s="7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D20" s="8" t="s">
         <v>39</v>
@@ -985,7 +988,7 @@
       <c r="A21" s="23"/>
       <c r="B21" s="23"/>
       <c r="C21" s="9" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D21" s="8" t="s">
         <v>11</v>
@@ -1003,7 +1006,7 @@
       <c r="A22" s="23"/>
       <c r="B22" s="23"/>
       <c r="C22" s="9" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D22" s="8" t="s">
         <v>42</v>
@@ -1021,7 +1024,7 @@
       <c r="A23" s="23"/>
       <c r="B23" s="23"/>
       <c r="C23" s="9" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="D23" s="8" t="s">
         <v>33</v>
@@ -1039,7 +1042,7 @@
       <c r="A24" s="23"/>
       <c r="B24" s="23"/>
       <c r="C24" s="9" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D24" s="8" t="s">
         <v>35</v>
@@ -1057,7 +1060,7 @@
       <c r="A25" s="23"/>
       <c r="B25" s="23"/>
       <c r="C25" s="9" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="D25" s="8" t="s">
         <v>34</v>

</xml_diff>

<commit_message>
Author           : Pooja Sharma Files Added      : PoojaSharma.xlsx Description      : Updated the previous existing file PoojaSharma.xlsx
</commit_message>
<xml_diff>
--- a/TeamDetails/TasksBreakDown/PoojaSharma.xlsx
+++ b/TeamDetails/TasksBreakDown/PoojaSharma.xlsx
@@ -683,8 +683,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -852,10 +852,12 @@
       <c r="E13" s="7">
         <v>2</v>
       </c>
-      <c r="F13" s="17"/>
+      <c r="F13" s="17">
+        <v>2</v>
+      </c>
       <c r="G13" s="17">
         <f>E13-F13</f>
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -870,10 +872,12 @@
       <c r="E14" s="7">
         <v>1</v>
       </c>
-      <c r="F14" s="17"/>
+      <c r="F14" s="17">
+        <v>1</v>
+      </c>
       <c r="G14" s="17">
         <f t="shared" ref="G14:G63" si="0">E14-F14</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -888,10 +892,12 @@
       <c r="E15" s="7">
         <v>1</v>
       </c>
-      <c r="F15" s="17"/>
+      <c r="F15" s="17">
+        <v>1</v>
+      </c>
       <c r="G15" s="17">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -906,10 +912,12 @@
       <c r="E16" s="7">
         <v>1</v>
       </c>
-      <c r="F16" s="17"/>
+      <c r="F16" s="17">
+        <v>1</v>
+      </c>
       <c r="G16" s="17">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
@@ -924,10 +932,12 @@
       <c r="E17" s="7">
         <v>2</v>
       </c>
-      <c r="F17" s="17"/>
+      <c r="F17" s="17">
+        <v>2</v>
+      </c>
       <c r="G17" s="17">
         <f t="shared" ref="G17:G18" si="1">E17-F17</f>
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Author           : Pooja Sharma Files modified   : PoojaSharma.xlsx Description      : modified the previous existing file PoojaSharma.xlsx
</commit_message>
<xml_diff>
--- a/TeamDetails/TasksBreakDown/PoojaSharma.xlsx
+++ b/TeamDetails/TasksBreakDown/PoojaSharma.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="49">
   <si>
     <t>Story ID</t>
   </si>
@@ -225,6 +225,18 @@
   </si>
   <si>
     <t>Styling</t>
+  </si>
+  <si>
+    <t>Total =</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>In QA</t>
   </si>
 </sst>
 </file>
@@ -277,7 +289,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -320,8 +332,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF7C80"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -344,11 +362,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -401,6 +456,45 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -411,6 +505,8 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFF7C80"/>
+      <color rgb="FFFF5050"/>
       <color rgb="FFFFCCFF"/>
       <color rgb="FFFF9966"/>
       <color rgb="FFFF99FF"/>
@@ -696,8 +792,8 @@
   </sheetPr>
   <dimension ref="A1:I61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -708,9 +804,10 @@
     <col min="5" max="5" width="14" customWidth="1"/>
     <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -729,11 +826,14 @@
       <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="26" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="H1" s="25" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="12"/>
       <c r="B2" s="12"/>
       <c r="C2" s="12"/>
@@ -746,8 +846,11 @@
         <f>E2-F2</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H2" s="27" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="12"/>
       <c r="B3" s="12"/>
       <c r="C3" s="12"/>
@@ -755,8 +858,9 @@
       <c r="E3" s="15"/>
       <c r="F3" s="16"/>
       <c r="G3" s="16"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H3" s="12"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="12"/>
       <c r="B4" s="12"/>
       <c r="C4" s="12"/>
@@ -766,8 +870,11 @@
       <c r="E4" s="15"/>
       <c r="F4" s="16"/>
       <c r="G4" s="16"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H4" s="31" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="12"/>
       <c r="B5" s="12"/>
       <c r="C5" s="12"/>
@@ -777,8 +884,9 @@
       <c r="E5" s="15"/>
       <c r="F5" s="16"/>
       <c r="G5" s="16"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H5" s="32"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="12"/>
       <c r="B6" s="12"/>
       <c r="C6" s="12"/>
@@ -788,8 +896,9 @@
       <c r="E6" s="15"/>
       <c r="F6" s="16"/>
       <c r="G6" s="16"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H6" s="33"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="12"/>
       <c r="B7" s="12"/>
       <c r="C7" s="12"/>
@@ -799,8 +908,9 @@
       <c r="E7" s="15"/>
       <c r="F7" s="16"/>
       <c r="G7" s="16"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H7" s="12"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="12"/>
       <c r="B8" s="12"/>
       <c r="C8" s="12"/>
@@ -808,8 +918,9 @@
       <c r="E8" s="15"/>
       <c r="F8" s="16"/>
       <c r="G8" s="16"/>
-    </row>
-    <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="H8" s="12"/>
+    </row>
+    <row r="9" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="12"/>
       <c r="B9" s="12"/>
       <c r="C9" s="12"/>
@@ -819,8 +930,11 @@
       <c r="E9" s="15"/>
       <c r="F9" s="16"/>
       <c r="G9" s="16"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H9" s="27" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="12"/>
       <c r="B10" s="12"/>
       <c r="C10" s="12"/>
@@ -828,8 +942,9 @@
       <c r="E10" s="15"/>
       <c r="F10" s="16"/>
       <c r="G10" s="16"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H10" s="12"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="12"/>
       <c r="B11" s="12"/>
       <c r="C11" s="12"/>
@@ -839,12 +954,15 @@
       <c r="E11" s="15"/>
       <c r="F11" s="16"/>
       <c r="G11" s="16"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="22" t="s">
+      <c r="H11" s="27" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="22">
+      <c r="B12" s="29">
         <v>22</v>
       </c>
       <c r="C12" s="5" t="s">
@@ -859,14 +977,17 @@
       <c r="F12" s="11">
         <v>2</v>
       </c>
-      <c r="G12" s="18">
+      <c r="G12" s="22">
         <f>E12-F12</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="22"/>
-      <c r="B13" s="22"/>
+      <c r="H12" s="34" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="29"/>
+      <c r="B13" s="29"/>
       <c r="C13" s="5" t="s">
         <v>13</v>
       </c>
@@ -876,15 +997,18 @@
       <c r="E13" s="5">
         <v>1</v>
       </c>
-      <c r="F13" s="11"/>
-      <c r="G13" s="18">
+      <c r="F13" s="11">
+        <v>1</v>
+      </c>
+      <c r="G13" s="22">
         <f t="shared" ref="G13:G27" si="0">E13-F13</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="22"/>
-      <c r="B14" s="22"/>
+        <v>0</v>
+      </c>
+      <c r="H13" s="35"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="29"/>
+      <c r="B14" s="29"/>
       <c r="C14" s="5" t="s">
         <v>14</v>
       </c>
@@ -897,14 +1021,15 @@
       <c r="F14" s="11">
         <v>1</v>
       </c>
-      <c r="G14" s="18">
+      <c r="G14" s="22">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="22"/>
-      <c r="B15" s="22"/>
+      <c r="H14" s="35"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="29"/>
+      <c r="B15" s="29"/>
       <c r="C15" s="5" t="s">
         <v>15</v>
       </c>
@@ -917,14 +1042,15 @@
       <c r="F15" s="11">
         <v>1</v>
       </c>
-      <c r="G15" s="18">
+      <c r="G15" s="22">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="22"/>
-      <c r="B16" s="22"/>
+      <c r="H15" s="35"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="29"/>
+      <c r="B16" s="29"/>
       <c r="C16" s="5" t="s">
         <v>16</v>
       </c>
@@ -937,14 +1063,15 @@
       <c r="F16" s="11">
         <v>2</v>
       </c>
-      <c r="G16" s="18">
+      <c r="G16" s="22">
         <f t="shared" ref="G16:G17" si="1">E16-F16</f>
         <v>0</v>
       </c>
+      <c r="H16" s="35"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="22"/>
-      <c r="B17" s="22"/>
+      <c r="A17" s="29"/>
+      <c r="B17" s="29"/>
       <c r="C17" s="5" t="s">
         <v>17</v>
       </c>
@@ -957,14 +1084,15 @@
       <c r="F17" s="11">
         <v>1</v>
       </c>
-      <c r="G17" s="18">
+      <c r="G17" s="22">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
+      <c r="H17" s="35"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="22"/>
-      <c r="B18" s="22"/>
+      <c r="A18" s="29"/>
+      <c r="B18" s="29"/>
       <c r="C18" s="5" t="s">
         <v>18</v>
       </c>
@@ -977,14 +1105,15 @@
       <c r="F18" s="11">
         <v>1</v>
       </c>
-      <c r="G18" s="18">
+      <c r="G18" s="22">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="H18" s="36"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="22"/>
-      <c r="B19" s="22"/>
+      <c r="A19" s="29"/>
+      <c r="B19" s="29"/>
       <c r="C19" s="5" t="s">
         <v>19</v>
       </c>
@@ -997,14 +1126,15 @@
       <c r="F19" s="11">
         <v>1</v>
       </c>
-      <c r="G19" s="18">
-        <v>1</v>
-      </c>
+      <c r="G19" s="22">
+        <v>1</v>
+      </c>
+      <c r="H19" s="11"/>
       <c r="I19" s="4"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="22"/>
-      <c r="B20" s="22"/>
+      <c r="A20" s="29"/>
+      <c r="B20" s="29"/>
       <c r="C20" s="18" t="s">
         <v>20</v>
       </c>
@@ -1015,14 +1145,15 @@
         <v>6</v>
       </c>
       <c r="F20" s="11"/>
-      <c r="G20" s="18">
+      <c r="G20" s="22">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
+      <c r="H20" s="11"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="22"/>
-      <c r="B21" s="22"/>
+      <c r="A21" s="29"/>
+      <c r="B21" s="29"/>
       <c r="C21" s="18" t="s">
         <v>21</v>
       </c>
@@ -1033,14 +1164,15 @@
         <v>2</v>
       </c>
       <c r="F21" s="11"/>
-      <c r="G21" s="18">
+      <c r="G21" s="22">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
+      <c r="H21" s="11"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="22"/>
-      <c r="B22" s="22"/>
+      <c r="A22" s="29"/>
+      <c r="B22" s="29"/>
       <c r="C22" s="18" t="s">
         <v>26</v>
       </c>
@@ -1051,14 +1183,15 @@
         <v>1</v>
       </c>
       <c r="F22" s="11"/>
-      <c r="G22" s="18">
+      <c r="G22" s="22">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
+      <c r="H22" s="11"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="22"/>
-      <c r="B23" s="22"/>
+      <c r="A23" s="29"/>
+      <c r="B23" s="29"/>
       <c r="C23" s="18" t="s">
         <v>27</v>
       </c>
@@ -1069,14 +1202,15 @@
         <v>1</v>
       </c>
       <c r="F23" s="11"/>
-      <c r="G23" s="18">
+      <c r="G23" s="22">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
+      <c r="H23" s="11"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="22"/>
-      <c r="B24" s="22"/>
+      <c r="A24" s="29"/>
+      <c r="B24" s="29"/>
       <c r="C24" s="18" t="s">
         <v>35</v>
       </c>
@@ -1087,16 +1221,17 @@
         <v>2</v>
       </c>
       <c r="F24" s="11"/>
-      <c r="G24" s="18">
+      <c r="G24" s="22">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
+      <c r="H24" s="11"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="23" t="s">
+      <c r="A25" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="B25" s="23">
+      <c r="B25" s="30">
         <v>10</v>
       </c>
       <c r="C25" s="8" t="s">
@@ -1111,14 +1246,17 @@
       <c r="F25" s="10">
         <v>4</v>
       </c>
-      <c r="G25" s="17">
+      <c r="G25" s="23">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="H25" s="23" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="23"/>
-      <c r="B26" s="23"/>
+      <c r="A26" s="30"/>
+      <c r="B26" s="30"/>
       <c r="C26" s="8" t="s">
         <v>13</v>
       </c>
@@ -1129,14 +1267,15 @@
         <v>4</v>
       </c>
       <c r="F26" s="10"/>
-      <c r="G26" s="17">
+      <c r="G26" s="23">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
+      <c r="H26" s="10"/>
     </row>
     <row r="27" spans="1:9" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="23"/>
-      <c r="B27" s="23"/>
+      <c r="A27" s="30"/>
+      <c r="B27" s="30"/>
       <c r="C27" s="17" t="s">
         <v>14</v>
       </c>
@@ -1149,10 +1288,11 @@
       <c r="F27" s="10">
         <v>1</v>
       </c>
-      <c r="G27" s="17">
+      <c r="G27" s="23">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
+      <c r="H27" s="10"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="20"/>
@@ -1160,8 +1300,13 @@
       <c r="C28" s="20"/>
       <c r="D28" s="21"/>
       <c r="E28" s="20"/>
-      <c r="F28" s="20"/>
-      <c r="G28" s="20"/>
+      <c r="F28" s="24" t="s">
+        <v>45</v>
+      </c>
+      <c r="G28" s="28">
+        <f>SUM(G12:G27)</f>
+        <v>18</v>
+      </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="20"/>
@@ -1461,11 +1606,13 @@
       <c r="G61" s="20"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="6">
     <mergeCell ref="A12:A24"/>
     <mergeCell ref="B12:B24"/>
     <mergeCell ref="A25:A27"/>
     <mergeCell ref="B25:B27"/>
+    <mergeCell ref="H4:H6"/>
+    <mergeCell ref="H12:H18"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>